<commit_message>
Addition of Container Comment column to Container Creation Template.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_v4_2_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_v4_2_0.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Container Creation Template</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">Parent Container Coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Container Comment</t>
   </si>
   <si>
     <t xml:space="preserve">Tube box 3x3</t>
@@ -467,18 +470,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="22.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="76.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="9.33"/>
   </cols>
   <sheetData>
@@ -512,7 +515,7 @@
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
@@ -528,97 +531,113 @@
       <c r="E7" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
@@ -626,6 +645,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
@@ -633,6 +653,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
@@ -640,6 +661,7 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
@@ -647,6 +669,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
@@ -654,6 +677,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
@@ -661,6 +685,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
@@ -668,6 +693,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
@@ -675,6 +701,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
@@ -682,6 +709,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
@@ -689,6 +717,7 @@
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
@@ -696,6 +725,7 @@
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
@@ -703,6 +733,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
@@ -710,6 +741,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
@@ -717,6 +749,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
@@ -724,6 +757,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
@@ -731,6 +765,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
@@ -738,6 +773,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
@@ -745,6 +781,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
@@ -752,6 +789,7 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
@@ -759,6 +797,7 @@
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
@@ -766,6 +805,7 @@
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
@@ -773,6 +813,7 @@
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
@@ -780,6 +821,7 @@
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="8"/>
@@ -787,6 +829,7 @@
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
@@ -794,6 +837,7 @@
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
@@ -801,6 +845,7 @@
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
@@ -808,6 +853,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
@@ -815,6 +861,7 @@
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
@@ -822,6 +869,7 @@
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
@@ -829,6 +877,7 @@
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
@@ -836,6 +885,7 @@
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="8"/>
@@ -843,6 +893,7 @@
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="8"/>
@@ -850,6 +901,7 @@
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="8"/>
@@ -857,6 +909,7 @@
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
@@ -864,6 +917,7 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
@@ -871,6 +925,7 @@
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
@@ -878,6 +933,7 @@
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
@@ -885,6 +941,7 @@
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="8"/>
@@ -892,6 +949,7 @@
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="8"/>
@@ -899,6 +957,7 @@
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
@@ -906,6 +965,7 @@
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="8"/>
@@ -913,6 +973,7 @@
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="8"/>
@@ -920,6 +981,7 @@
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>
@@ -927,6 +989,7 @@
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="8"/>
@@ -934,6 +997,7 @@
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="8"/>
@@ -941,6 +1005,7 @@
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="8"/>
@@ -948,6 +1013,7 @@
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="8"/>
@@ -955,6 +1021,7 @@
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="8"/>
@@ -962,6 +1029,7 @@
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="8"/>
@@ -969,6 +1037,7 @@
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="8"/>
@@ -976,6 +1045,7 @@
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="8"/>
@@ -983,6 +1053,7 @@
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="8"/>
@@ -990,6 +1061,7 @@
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="8"/>
@@ -997,6 +1069,7 @@
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="8"/>
@@ -1004,6 +1077,7 @@
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="8"/>
@@ -1011,6 +1085,7 @@
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="8"/>
@@ -1018,6 +1093,7 @@
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="8"/>
@@ -1025,6 +1101,7 @@
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
       <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="8"/>
@@ -1032,6 +1109,7 @@
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="8"/>
@@ -1039,6 +1117,7 @@
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="8"/>
@@ -1046,6 +1125,7 @@
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="8"/>
@@ -1053,6 +1133,7 @@
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="8"/>
@@ -1060,6 +1141,7 @@
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="8"/>
@@ -1067,6 +1149,7 @@
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="8"/>
@@ -1074,6 +1157,7 @@
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="8"/>
@@ -1081,6 +1165,7 @@
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="8"/>
@@ -1088,6 +1173,7 @@
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="8"/>
@@ -1095,6 +1181,7 @@
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="8"/>
@@ -1102,6 +1189,7 @@
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="8"/>
@@ -1109,6 +1197,7 @@
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="8"/>
@@ -1116,6 +1205,7 @@
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="8"/>
@@ -1123,6 +1213,7 @@
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
       <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="8"/>
@@ -1130,6 +1221,7 @@
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="8"/>
@@ -1137,6 +1229,7 @@
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="8"/>
@@ -1144,6 +1237,7 @@
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="8"/>
@@ -1151,6 +1245,7 @@
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="8"/>
@@ -1158,6 +1253,7 @@
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="8"/>
@@ -1165,6 +1261,7 @@
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="8"/>
@@ -1172,6 +1269,7 @@
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="8"/>
@@ -1179,6 +1277,7 @@
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="8"/>
@@ -1186,6 +1285,7 @@
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="8"/>
@@ -1193,6 +1293,7 @@
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
       <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="8"/>
@@ -1200,6 +1301,7 @@
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
       <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="8"/>
@@ -1207,6 +1309,7 @@
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
       <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="8"/>
@@ -1214,6 +1317,7 @@
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
       <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="8"/>
@@ -1221,6 +1325,7 @@
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
       <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="11"/>
@@ -1228,6 +1333,7 @@
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4"/>
@@ -4826,10 +4932,10 @@
   <dimension ref="A1:A1013"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>
@@ -4842,132 +4948,132 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Renamed column Comment to match other templates column.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_v4_2_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_v4_2_0.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Parent Container Coordinates</t>
   </si>
   <si>
-    <t xml:space="preserve">Container Comment</t>
+    <t xml:space="preserve">Comment</t>
   </si>
   <si>
     <t xml:space="preserve">Tube box 3x3</t>
@@ -476,7 +476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="22.33"/>
@@ -4935,7 +4935,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>

</xml_diff>